<commit_message>
case sheet comments for approval
</commit_message>
<xml_diff>
--- a/APIs.xlsx
+++ b/APIs.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\F Drive\10Soft\dental\10SoftClinic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\10Soft-Dental-Clinic\10SoftClinic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCFB11B-05DD-4E77-BAE2-CD2B910716BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C32AAF5E-5F07-4CE6-9D4A-2B8A8542038E}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,12 +29,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>USER</author>
   </authors>
   <commentList>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{65716A2F-E2AA-474B-82BA-A64FFE00365A}">
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{263ABDDB-9C8C-4C8A-A5A2-11B89EF2BC2C}">
+    <comment ref="I3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -92,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{0EBEE5D4-21A6-4D02-A82F-94C80BE502B7}">
+    <comment ref="I4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -121,7 +120,108 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{E2BB3F94-9327-4CCF-9996-708661483F7C}">
+    <comment ref="F6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Use GetDentalAdultTreatmentMaster for chief complaint dropdown this is get call search
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Sample Object
+{
+"DentalAdultMainId":24,
+ "IsSentforCaseStudy":true,
+  "CaseAssignedStudentId":6
+}</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Sample object
+{
+"DentalAdultMainId":24,
+ "ApprovedStatus":"Approved"
+}</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Send Case sheet for approval
+Example: 
+{
+"DentalAdultMainId":24,
+ "IsSentforApproval":true
+}</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>Adult Treatment</t>
   </si>
@@ -249,12 +349,18 @@
   </si>
   <si>
     <t>Approvals</t>
+  </si>
+  <si>
+    <t>after screening</t>
+  </si>
+  <si>
+    <t>Child Treatment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -298,7 +404,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,6 +414,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,12 +494,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -391,9 +512,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,26 +829,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D9951C-75C9-4066-BF39-16070777F30C}">
-  <dimension ref="B1:I12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" customWidth="1"/>
+    <col min="6" max="6" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
         <v>15</v>
@@ -740,23 +862,26 @@
       <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="6"/>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="7"/>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
@@ -775,8 +900,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="6"/>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
       <c r="C4" s="1" t="s">
         <v>29</v>
       </c>
@@ -793,8 +918,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="6"/>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="7"/>
       <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
@@ -809,8 +934,8 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="6"/>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -825,22 +950,22 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="6"/>
-      <c r="C7" s="1" t="s">
+    <row r="7" spans="2:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+      <c r="C7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="6"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
@@ -853,26 +978,26 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="6"/>
-      <c r="C9" s="1" t="s">
+    <row r="9" spans="2:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
@@ -883,7 +1008,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
@@ -901,7 +1026,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
@@ -919,9 +1044,149 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="H16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+      <c r="C18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+      <c r="C19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="2:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="2:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+      <c r="C23" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:B10"/>
+    <mergeCell ref="B16:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>